<commit_message>
Implemented story 2, 4 and 10. Created general ValidationService
</commit_message>
<xml_diff>
--- a/api_structure.xlsx
+++ b/api_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andreeas Firoiu\Desktop\eurder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EA73928-FEC7-451C-B26B-1BEAD4161792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBAC7DA-40A2-452B-8F13-6C3B1EE54A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3E4EB9F0-576F-4F3D-9C6E-D4C73761F290}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3E4EB9F0-576F-4F3D-9C6E-D4C73761F290}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
   <si>
     <t>Resource</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>Order, item groups, total amount</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -395,7 +401,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -442,6 +448,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Goed 2" xfId="2" xr:uid="{864CBD22-5C24-47DC-9FD3-3897AC86D9C7}"/>
@@ -449,7 +462,18 @@
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{E8B37425-C93D-4E59-816D-5624C5196938}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -759,360 +783,387 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08587191-8D21-4B5D-9320-73505106E411}">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.88671875" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="26.77734375" customWidth="1"/>
-    <col min="8" max="8" width="29.33203125" customWidth="1"/>
-    <col min="11" max="11" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.77734375" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="8" max="8" width="26.77734375" customWidth="1"/>
+    <col min="9" max="9" width="29.33203125" customWidth="1"/>
+    <col min="12" max="12" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:15" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="H3" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="I3" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="N3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="O3" s="7"/>
+    </row>
+    <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="C4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="D4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="G4" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="H4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="22">
+      <c r="I4" s="26">
         <v>7</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
-    </row>
-    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="O4" s="7"/>
+    </row>
+    <row r="5" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="C5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="D5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="20"/>
+      <c r="F5" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="G5" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="H5" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="20">
+      <c r="I5" s="27">
         <v>8</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="L5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="O5" s="7"/>
+    </row>
+    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C6" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="D6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="E6" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="F6" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="G6" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="H6" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="20">
+      <c r="I6" s="27">
         <v>2</v>
       </c>
-      <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="7"/>
+      <c r="O6" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="C7" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="D7" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="E7" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="F7" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="H7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="20">
+      <c r="I7" s="27">
         <v>4</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="18" t="s">
+      <c r="L7" s="7"/>
+      <c r="M7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="7"/>
       <c r="N7" s="7"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="O7" s="7"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="C8" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="D8" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="17" t="s">
+      <c r="I8" s="27"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="M8" s="15"/>
-      <c r="N8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="N8" s="15"/>
+      <c r="O8" s="14"/>
+    </row>
+    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="C9" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="D9" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="20"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="20"/>
+      <c r="G9" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20">
+      <c r="H9" s="20"/>
+      <c r="I9" s="27">
         <v>10</v>
       </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="15"/>
+      <c r="L9" s="7"/>
       <c r="M9" s="15"/>
-      <c r="N9" s="16" t="s">
+      <c r="N9" s="15"/>
+      <c r="O9" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="C10" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="D10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="20"/>
+      <c r="F10" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="G10" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="H10" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="20">
+      <c r="I10" s="27">
         <v>10</v>
       </c>
-      <c r="K10" s="7"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="14"/>
-    </row>
-    <row r="11" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="M10" s="7"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="14"/>
+    </row>
+    <row r="11" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="C11" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="D11" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="E11" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="F11" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="G11" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="H11" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="20">
+      <c r="I11" s="27">
         <v>3</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="12" t="s">
+      <c r="L11" s="7"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="13"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
+      <c r="O11" s="13"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -1120,9 +1171,9 @@
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
+      <c r="I12" s="20"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
@@ -1130,9 +1181,9 @@
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
+      <c r="I13" s="20"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
@@ -1140,9 +1191,9 @@
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
@@ -1150,9 +1201,9 @@
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
+      <c r="I15" s="20"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B16" s="20"/>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
@@ -1160,9 +1211,9 @@
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
@@ -1170,9 +1221,9 @@
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
+      <c r="I17" s="20"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
@@ -1180,9 +1231,9 @@
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
+      <c r="I18" s="20"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
@@ -1190,9 +1241,9 @@
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
+      <c r="I19" s="20"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
@@ -1200,9 +1251,9 @@
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
+      <c r="I20" s="20"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
@@ -1210,9 +1261,9 @@
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
+      <c r="I21" s="20"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
@@ -1220,9 +1271,9 @@
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
+      <c r="I22" s="20"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
@@ -1230,9 +1281,9 @@
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
+      <c r="I23" s="20"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
@@ -1240,9 +1291,9 @@
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
+      <c r="I24" s="20"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
@@ -1250,9 +1301,9 @@
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
+      <c r="I25" s="20"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
@@ -1260,9 +1311,9 @@
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
@@ -1270,9 +1321,9 @@
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
@@ -1280,9 +1331,9 @@
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
@@ -1290,9 +1341,9 @@
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
@@ -1300,9 +1351,9 @@
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
+      <c r="I30" s="20"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
@@ -1310,9 +1361,9 @@
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
+      <c r="I31" s="20"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
       <c r="D32" s="20"/>
@@ -1320,9 +1371,9 @@
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="20"/>
+      <c r="I32" s="20"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
       <c r="D33" s="20"/>
@@ -1330,9 +1381,9 @@
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="20"/>
+      <c r="I33" s="20"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
@@ -1340,9 +1391,9 @@
       <c r="F34" s="20"/>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="20"/>
+      <c r="I34" s="20"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
       <c r="D35" s="20"/>
@@ -1350,9 +1401,9 @@
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
       <c r="H35" s="20"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="20"/>
+      <c r="I35" s="20"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
@@ -1360,9 +1411,9 @@
       <c r="F36" s="20"/>
       <c r="G36" s="20"/>
       <c r="H36" s="20"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="20"/>
+      <c r="I36" s="20"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
       <c r="D37" s="20"/>
@@ -1370,9 +1421,9 @@
       <c r="F37" s="20"/>
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="20"/>
+      <c r="I37" s="20"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
@@ -1380,9 +1431,9 @@
       <c r="F38" s="20"/>
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="20"/>
+      <c r="I38" s="20"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
       <c r="D39" s="20"/>
@@ -1390,9 +1441,9 @@
       <c r="F39" s="20"/>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="20"/>
+      <c r="I39" s="20"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
       <c r="D40" s="20"/>
@@ -1400,9 +1451,9 @@
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
       <c r="H40" s="20"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="20"/>
+      <c r="I40" s="20"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
       <c r="D41" s="20"/>
@@ -1410,9 +1461,9 @@
       <c r="F41" s="20"/>
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="20"/>
+      <c r="I41" s="20"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
       <c r="D42" s="20"/>
@@ -1420,9 +1471,9 @@
       <c r="F42" s="20"/>
       <c r="G42" s="20"/>
       <c r="H42" s="20"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="20"/>
+      <c r="I42" s="20"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
       <c r="D43" s="20"/>
@@ -1430,9 +1481,9 @@
       <c r="F43" s="20"/>
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="20"/>
+      <c r="I43" s="20"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
@@ -1440,9 +1491,9 @@
       <c r="F44" s="20"/>
       <c r="G44" s="20"/>
       <c r="H44" s="20"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="20"/>
+      <c r="I44" s="20"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="20"/>
       <c r="C45" s="20"/>
       <c r="D45" s="20"/>
@@ -1450,9 +1501,9 @@
       <c r="F45" s="20"/>
       <c r="G45" s="20"/>
       <c r="H45" s="20"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="20"/>
+      <c r="I45" s="20"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" s="20"/>
       <c r="C46" s="20"/>
       <c r="D46" s="20"/>
@@ -1460,9 +1511,9 @@
       <c r="F46" s="20"/>
       <c r="G46" s="20"/>
       <c r="H46" s="20"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="20"/>
+      <c r="I46" s="20"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
@@ -1470,9 +1521,9 @@
       <c r="F47" s="20"/>
       <c r="G47" s="20"/>
       <c r="H47" s="20"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="20"/>
+      <c r="I47" s="20"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" s="20"/>
       <c r="C48" s="20"/>
       <c r="D48" s="20"/>
@@ -1480,9 +1531,9 @@
       <c r="F48" s="20"/>
       <c r="G48" s="20"/>
       <c r="H48" s="20"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="20"/>
+      <c r="I48" s="20"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" s="20"/>
       <c r="C49" s="20"/>
       <c r="D49" s="20"/>
@@ -1490,9 +1541,9 @@
       <c r="F49" s="20"/>
       <c r="G49" s="20"/>
       <c r="H49" s="20"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="20"/>
+      <c r="I49" s="20"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
       <c r="D50" s="20"/>
@@ -1500,9 +1551,9 @@
       <c r="F50" s="20"/>
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="20"/>
+      <c r="I50" s="20"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
       <c r="D51" s="20"/>
@@ -1510,8 +1561,14 @@
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
       <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A3:A30">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>